<commit_message>
✨Novos produtos no index
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D400A4C-2BD6-4CA9-BA99-0E21C8AEFEC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACFD702-C239-4DF5-8508-63329F1EA47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0C260EFA-34F1-469A-9DCE-051C064AD26C}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="152">
   <si>
     <t>ID</t>
   </si>
@@ -212,9 +212,6 @@
     <t>'Brinco',</t>
   </si>
   <si>
-    <t>'Colar',</t>
-  </si>
-  <si>
     <t>'Pequeno',</t>
   </si>
   <si>
@@ -495,6 +492,24 @@
   </si>
   <si>
     <t>'Porta Joias Dauphine',</t>
+  </si>
+  <si>
+    <t>'Pulseira, Mais Vendidos',</t>
+  </si>
+  <si>
+    <t>'Brinco, Mais Vendidos',</t>
+  </si>
+  <si>
+    <t>'Pulseira, Index',</t>
+  </si>
+  <si>
+    <t>'Colar, Index',</t>
+  </si>
+  <si>
+    <t>'Brinco, Index',</t>
+  </si>
+  <si>
+    <t>'Conjunto, Mais Vendidos',</t>
   </si>
 </sst>
 </file>
@@ -926,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9376D30-AA93-47B8-A013-E886A455A1C7}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -935,7 +950,7 @@
     <col min="1" max="1" width="8.88671875" customWidth="1"/>
     <col min="2" max="2" width="76.44140625" customWidth="1"/>
     <col min="3" max="3" width="68.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.44140625" customWidth="1"/>
     <col min="6" max="6" width="18.21875" customWidth="1"/>
     <col min="7" max="7" width="14.21875" customWidth="1"/>
@@ -978,16 +993,16 @@
         <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
@@ -999,7 +1014,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1007,19 +1022,19 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>10</v>
@@ -1028,7 +1043,7 @@
         <v>11</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -1036,16 +1051,16 @@
         <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>148</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>12</v>
@@ -1057,7 +1072,7 @@
         <v>11</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1065,10 +1080,10 @@
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>9</v>
@@ -1086,7 +1101,7 @@
         <v>11</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1094,19 +1109,19 @@
         <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>9</v>
+        <v>148</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>10</v>
@@ -1115,7 +1130,7 @@
         <v>11</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1123,19 +1138,19 @@
         <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>52</v>
+        <v>149</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>10</v>
@@ -1144,7 +1159,7 @@
         <v>11</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1152,19 +1167,19 @@
         <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>66</v>
+        <v>151</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>10</v>
@@ -1173,7 +1188,7 @@
         <v>11</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1181,19 +1196,19 @@
         <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>10</v>
@@ -1202,7 +1217,7 @@
         <v>11</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1210,10 +1225,10 @@
         <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>9</v>
@@ -1222,7 +1237,7 @@
         <v>12</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>10</v>
@@ -1231,7 +1246,7 @@
         <v>11</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1239,19 +1254,19 @@
         <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>52</v>
+        <v>149</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>10</v>
@@ -1260,7 +1275,7 @@
         <v>11</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1268,13 +1283,13 @@
         <v>23</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>9</v>
+        <v>148</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>12</v>
@@ -1289,7 +1304,7 @@
         <v>11</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1297,13 +1312,13 @@
         <v>24</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>52</v>
+        <v>149</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>12</v>
@@ -1318,7 +1333,7 @@
         <v>11</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1326,13 +1341,13 @@
         <v>49</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>12</v>
@@ -1347,7 +1362,7 @@
         <v>11</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1355,13 +1370,13 @@
         <v>48</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>12</v>
@@ -1376,7 +1391,7 @@
         <v>11</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1384,10 +1399,10 @@
         <v>47</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>9</v>
@@ -1405,7 +1420,7 @@
         <v>11</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1413,13 +1428,13 @@
         <v>46</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>52</v>
+        <v>149</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>12</v>
@@ -1434,7 +1449,7 @@
         <v>11</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1442,10 +1457,10 @@
         <v>45</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>51</v>
@@ -1457,13 +1472,13 @@
         <v>50</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1471,10 +1486,10 @@
         <v>44</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>51</v>
@@ -1486,13 +1501,13 @@
         <v>50</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1500,10 +1515,10 @@
         <v>43</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>51</v>
@@ -1515,13 +1530,13 @@
         <v>50</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1529,13 +1544,13 @@
         <v>42</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>51</v>
+        <v>147</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>12</v>
@@ -1544,13 +1559,13 @@
         <v>50</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1558,10 +1573,10 @@
         <v>41</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>51</v>
@@ -1573,13 +1588,13 @@
         <v>50</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -1587,10 +1602,10 @@
         <v>40</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>51</v>
@@ -1602,13 +1617,13 @@
         <v>50</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -1616,10 +1631,10 @@
         <v>39</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>51</v>
@@ -1631,13 +1646,13 @@
         <v>50</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -1645,13 +1660,13 @@
         <v>38</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>51</v>
+        <v>150</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>12</v>
@@ -1660,13 +1675,13 @@
         <v>50</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -1674,10 +1689,10 @@
         <v>37</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>51</v>
@@ -1689,13 +1704,13 @@
         <v>50</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1703,10 +1718,10 @@
         <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>51</v>
@@ -1718,13 +1733,13 @@
         <v>50</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1732,13 +1747,13 @@
         <v>35</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>51</v>
+        <v>150</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>12</v>
@@ -1747,13 +1762,13 @@
         <v>50</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1761,10 +1776,10 @@
         <v>34</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>51</v>
@@ -1773,16 +1788,16 @@
         <v>12</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -1790,10 +1805,10 @@
         <v>33</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>51</v>
@@ -1802,16 +1817,16 @@
         <v>12</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -1819,28 +1834,28 @@
         <v>32</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>51</v>
+        <v>150</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F31" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="H31" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -1848,10 +1863,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>51</v>
@@ -1863,13 +1878,13 @@
         <v>50</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -1877,10 +1892,10 @@
         <v>30</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>51</v>
@@ -1892,13 +1907,13 @@
         <v>50</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -1906,10 +1921,10 @@
         <v>29</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>51</v>
@@ -1921,13 +1936,13 @@
         <v>50</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1935,13 +1950,13 @@
         <v>28</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>51</v>
+        <v>150</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>12</v>
@@ -1950,13 +1965,13 @@
         <v>50</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -1964,13 +1979,13 @@
         <v>27</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>51</v>
+        <v>147</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>12</v>
@@ -1979,13 +1994,13 @@
         <v>50</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -1993,10 +2008,10 @@
         <v>26</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>51</v>
@@ -2008,13 +2023,13 @@
         <v>50</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -2022,28 +2037,28 @@
         <v>25</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="D38" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="G38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>